<commit_message>
Se creo la clase inventario con el metodo de leer inventario
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -13,7 +13,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -70,6 +70,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -91,6 +92,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,8 +137,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -273,99 +279,99 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.66"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>650</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -374,8 +380,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
250724 Se creo la clase inventario con el metodo de leer inventario
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -13,7 +13,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -70,6 +70,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -91,6 +92,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,8 +137,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -273,99 +279,99 @@
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.66"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>650</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -374,8 +380,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2025-08-06 -Se cambio el nombre del programa ManejoInventarioVentas.py -> MiTiendaApp.py -Se actualizo el nombre del inventario Inventario.xlsx -> Inventario_2.xlsx -Se Actualizaron los metodos <<agregar>> y <<leer>> -Se agrego manejo de excepciones FileNotFound en los metodos <<agregar>> y <<leer>> -Se actualizo el bloque de codigo <<Agregar roducto al inventario>>
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Inventario" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Splash Victoria Secret</t>
   </si>
   <si>
-    <t xml:space="preserve">und</t>
+    <t xml:space="preserve">unidades</t>
   </si>
   <si>
     <t xml:space="preserve">Splash Pink</t>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Esencia</t>
   </si>
   <si>
-    <t xml:space="preserve">ml</t>
+    <t xml:space="preserve">gramos</t>
   </si>
   <si>
     <t xml:space="preserve">Loción Possession</t>
@@ -276,7 +276,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
2025-09-06 -Se creo el metodo para vender productos -Se Cambio el nombre del programa de MiTiendaApp a TiendaApp
</commit_message>
<xml_diff>
--- a/Inventario.xlsx
+++ b/Inventario.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Inventario" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Precios" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t xml:space="preserve">Producto</t>
   </si>
@@ -29,6 +30,15 @@
   </si>
   <si>
     <t xml:space="preserve">Unidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precio Compra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precio Venta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilidad</t>
   </si>
   <si>
     <t xml:space="preserve">Splash Victoria Secret</t>
@@ -142,11 +152,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -275,13 +285,15 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -294,85 +306,103 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>8500</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>10000</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>36</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>8200</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>650</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>250</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>45</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -384,4 +414,152 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.56"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>8500</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>17000</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">C2-B2</f>
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>19000</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">C3-B3</f>
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>8200</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>16000</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">C4-B4</f>
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <f aca="false">C5-B5</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>14000</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>32000</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <f aca="false">C6-B6</f>
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>7400</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>15000</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <f aca="false">C7-B7</f>
+        <v>7600</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>7600</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>15000</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <f aca="false">C8-B8</f>
+        <v>7400</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12 Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>